<commit_message>
Changes:1.) Added Mauve Color - New Default Template Sheet.
</commit_message>
<xml_diff>
--- a/etc/defult-excel-template/default-template.xlsx
+++ b/etc/defult-excel-template/default-template.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9105" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="default-template-sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="default-template-sheet (1)" sheetId="2" r:id="rId1"/>
+    <sheet name="default-template-sheet (2)" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="144525"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,16 +20,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Sr No</t>
+  </si>
+  <si>
+    <t>Sr. No.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,8 +61,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -83,6 +94,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC3399"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -150,26 +167,6 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -178,6 +175,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -185,6 +206,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC3399"/>
+      <color rgb="FF660066"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -485,21 +512,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
@@ -511,123 +538,123 @@
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8">
-      <c r="B2" s="9"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3" spans="2:8">
-      <c r="B3" s="1" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="3">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="3">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="B6" s="3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
         <v>3</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="B7" s="3">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
         <v>4</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="2:8">
-      <c r="B8" s="3">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
         <v>5</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="B9" s="3">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
         <v>6</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="2:8">
-      <c r="B10" s="3">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
         <v>7</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="B11" s="3">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
         <v>8</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="2:8">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="7"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -636,4 +663,139 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <f>B3+1</f>
+        <v>2</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes:1.) Default Excel Template
</commit_message>
<xml_diff>
--- a/etc/defult-excel-template/default-template.xlsx
+++ b/etc/defult-excel-template/default-template.xlsx
@@ -20,19 +20,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Sr No</t>
   </si>
   <si>
     <t>Sr. No.</t>
   </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Birth-Day</t>
+  </si>
+  <si>
+    <t>Shri Shri</t>
+  </si>
+  <si>
+    <t>Priyanka G</t>
+  </si>
+  <si>
+    <t>Father In Law</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,8 +83,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF181818"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,8 +121,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F4F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -161,12 +194,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF686868"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF686868"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF686868"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF686868"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -176,29 +248,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -208,6 +262,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9900CC"/>
       <color rgb="FFCC3399"/>
       <color rgb="FF660066"/>
     </mruColors>
@@ -512,7 +567,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -539,122 +594,122 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="10"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="6">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
+      <c r="B5" s="3">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="8"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
+      <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="8"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
+      <c r="B8" s="3">
         <v>5</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
+      <c r="B9" s="3">
         <v>6</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
+      <c r="B10" s="3">
         <v>7</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
+      <c r="B11" s="3">
         <v>8</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="8"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="8"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -667,132 +722,142 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H11"/>
+  <dimension ref="B2:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="6">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="6">
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="12">
+        <v>3</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="2:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3">
         <f>B3+1</f>
         <v>2</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
+      <c r="C4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
+      <c r="F4" s="13">
+        <v>9</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="2:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
         <v>4</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
+      <c r="C5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
+      <c r="E5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="13">
+        <v>17</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
         <v>6</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
         <v>7</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
         <v>8</v>
       </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>